<commit_message>
finalized the evaporation time series analysis and added small changes to data and temperature time series analysis
</commit_message>
<xml_diff>
--- a/data/timeseries/FortStockton, NW/FortStockton, Evap.xlsx
+++ b/data/timeseries/FortStockton, NW/FortStockton, Evap.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans-\Documents\Master\1.Semester\ASTD\FinalAssignment\data\timeseries\FortStockton, NW\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCDBA95-E812-4834-9463-9778ACC0FF11}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FortStockton, Evap" sheetId="1" r:id="rId1"/>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -886,10 +887,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3474"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A378" workbookViewId="0">
+      <selection activeCell="G395" sqref="G395"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -9952,7 +9955,7 @@
         <v>18716</v>
       </c>
       <c r="G394">
-        <v>83.8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="395" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>